<commit_message>
ver 1.1 2020/08/09 [430424/32244]   added BH1750FVI (lux) sensor  - prepared (but not moved yet!) new HTML templates
</commit_message>
<xml_diff>
--- a/WeatherStation2_webserver/WeatherStation.xlsx
+++ b/WeatherStation2_webserver/WeatherStation.xlsx
@@ -1,41 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WeatherStation2_webserver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088A1EDA-804C-46CC-B57D-D3E516EC1252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B258420-99D3-4529-AAA4-C76B3F79CC00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B0C9A41E-2C7E-4A7A-8B40-CD68F4668925}"/>
   </bookViews>
   <sheets>
-    <sheet name="list" sheetId="2" r:id="rId1"/>
-    <sheet name="Capacitive Rain" sheetId="1" r:id="rId2"/>
-    <sheet name="mlx" sheetId="3" r:id="rId3"/>
+    <sheet name="wire (test)" sheetId="4" r:id="rId1"/>
+    <sheet name="list" sheetId="2" r:id="rId2"/>
+    <sheet name="Capacitive Rain" sheetId="1" r:id="rId3"/>
+    <sheet name="mlx" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
   <si>
     <t>Electrical Parameters</t>
   </si>
@@ -361,6 +354,9 @@
   </si>
   <si>
     <t>Спец. блок?</t>
+  </si>
+  <si>
+    <t>Test wire diagram</t>
   </si>
 </sst>
 </file>
@@ -574,6 +570,689 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>139200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>121150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Овал 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F032155-5DAF-486D-9566-4D383C3F6F65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1358400" y="514350"/>
+          <a:ext cx="1080000" cy="1080000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Прямоугольник 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A7EA6DD-A139-45DF-94E9-2466E7CCB49B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1841500" y="450850"/>
+          <a:ext cx="101600" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Овал 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6FC5C7C-3EB9-400A-BE0E-E1BDFCD68F0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1619250" y="755650"/>
+          <a:ext cx="133350" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Овал 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C45C16-1371-4985-9FBC-4E2CB029C09A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2012950" y="755650"/>
+          <a:ext cx="133350" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Овал 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C64CDBA1-2803-4C0B-9C73-EC6731E78067}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1619250" y="1187450"/>
+          <a:ext cx="133350" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Овал 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82C744F2-AF5E-4A03-80D7-13B269359CAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2012950" y="1187450"/>
+          <a:ext cx="133350" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Прямая соединительная линия 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E216321-4861-406D-8967-962E311840B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2336800" y="368300"/>
+          <a:ext cx="1930400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Прямая соединительная линия 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67228FA2-3F0B-4592-9588-2E45025D8F64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2120900" y="1841500"/>
+          <a:ext cx="2146300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Прямая соединительная линия 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5A98CA0-569A-4F4C-BF39-2FA915D61B68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1714500" y="1301750"/>
+          <a:ext cx="406400" cy="539750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Прямая соединительная линия 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{732F2615-1EE0-4B18-8BAC-144C1297E9A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1739900" y="368300"/>
+          <a:ext cx="609600" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Прямая соединительная линия 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96BE1C6B-841F-4F31-9EB5-BD6378AC57AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2159000" y="736600"/>
+          <a:ext cx="2146300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Прямая соединительная линия 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31B4734E-B5CF-45B9-8EC3-7C65F124AF54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2171700" y="1289050"/>
+          <a:ext cx="2146300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -638,7 +1317,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1000,11 +1679,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FE82ED-A626-4C51-9541-F900C0D39745}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E350CCA7-7452-459E-9649-8BA1D1792C0B}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1409,6 +2129,9 @@
       <c r="A27" s="20" t="s">
         <v>84</v>
       </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
       <c r="D27" s="20" t="s">
         <v>91</v>
       </c>
@@ -1426,6 +2149,9 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
       <c r="H28">
         <v>9</v>
       </c>
@@ -1479,7 +2205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C6D46C-1DF6-4DA4-BA65-59785C263F84}">
   <dimension ref="A4:N56"/>
   <sheetViews>
@@ -1925,7 +2651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB089DF1-9149-4C20-B4B4-0C866A8CD97C}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
[WeatherStatoin] HTML update 2.4: normalized pressure calc
</commit_message>
<xml_diff>
--- a/WeatherStation2_webserver/WeatherStation.xlsx
+++ b/WeatherStation2_webserver/WeatherStation.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WeatherStation2_webserver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko Boris\Documents\Arduino\WeatherStation2_webserver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B258420-99D3-4529-AAA4-C76B3F79CC00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B0C9A41E-2C7E-4A7A-8B40-CD68F4668925}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="38618" windowHeight="21218" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="wire (test)" sheetId="4" r:id="rId1"/>
     <sheet name="list" sheetId="2" r:id="rId2"/>
     <sheet name="Capacitive Rain" sheetId="1" r:id="rId3"/>
     <sheet name="mlx" sheetId="3" r:id="rId4"/>
+    <sheet name="давление" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
   <si>
     <t>Electrical Parameters</t>
   </si>
@@ -358,15 +358,36 @@
   <si>
     <t>Test wire diagram</t>
   </si>
+  <si>
+    <t>P=P_{0}e^{-Mgh/RT}</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>-Mgh/RT</t>
+  </si>
+  <si>
+    <t>e^{-Mgh/RT}</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,8 +450,24 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +516,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -507,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -551,9 +594,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1679,21 +1727,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FE82ED-A626-4C51-9541-F900C0D39745}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1704,7 +1752,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1720,22 +1768,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E350CCA7-7452-459E-9649-8BA1D1792C0B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27:B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="1" max="1" width="25.796875" customWidth="1"/>
+    <col min="2" max="2" width="13.265625" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="4" max="4" width="22.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B1" s="14" t="s">
         <v>66</v>
       </c>
@@ -1752,7 +1800,7 @@
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1770,7 +1818,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1790,7 +1838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="G4" s="17" t="s">
         <v>88</v>
       </c>
@@ -1807,7 +1855,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1833,7 +1881,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -1853,7 +1901,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="G7" s="17">
         <v>1</v>
       </c>
@@ -1864,7 +1912,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1884,12 +1932,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="I10" s="4" t="s">
         <v>76</v>
       </c>
@@ -1897,7 +1945,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H11">
         <v>1</v>
       </c>
@@ -1911,7 +1959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1931,7 +1979,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1951,7 +1999,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1965,7 +2013,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1979,7 +2027,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H16">
         <v>6</v>
       </c>
@@ -1987,7 +2035,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
@@ -1995,7 +2043,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>61</v>
       </c>
@@ -2012,7 +2060,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>62</v>
       </c>
@@ -2029,7 +2077,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H21">
         <v>2</v>
       </c>
@@ -2043,7 +2091,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H22">
         <v>3</v>
       </c>
@@ -2057,7 +2105,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>60</v>
       </c>
@@ -2080,7 +2128,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>63</v>
       </c>
@@ -2097,7 +2145,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H25">
         <v>6</v>
       </c>
@@ -2111,7 +2159,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H26">
         <v>7</v>
       </c>
@@ -2125,7 +2173,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="20" t="s">
         <v>84</v>
       </c>
@@ -2148,7 +2196,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>63</v>
       </c>
@@ -2159,7 +2207,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H29">
         <v>10</v>
       </c>
@@ -2167,7 +2215,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H30">
         <v>11</v>
       </c>
@@ -2175,7 +2223,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H31">
         <v>12</v>
       </c>
@@ -2183,7 +2231,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H32">
         <v>13</v>
       </c>
@@ -2191,7 +2239,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H33">
         <v>14</v>
       </c>
@@ -2206,16 +2254,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C6D46C-1DF6-4DA4-BA65-59785C263F84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="4" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2223,7 +2271,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2234,7 +2282,7 @@
       </c>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2245,7 +2293,7 @@
       </c>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2259,7 +2307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I15" t="s">
         <v>20</v>
       </c>
@@ -2276,7 +2324,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I16" t="s">
         <v>18</v>
       </c>
@@ -2297,7 +2345,7 @@
         <v>3.4285714285714284</v>
       </c>
     </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I17" t="s">
         <v>19</v>
       </c>
@@ -2318,7 +2366,7 @@
         <v>285.71428571428572</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="4" t="s">
         <v>21</v>
       </c>
@@ -2329,7 +2377,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" ht="72" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="7" t="s">
         <v>22</v>
       </c>
@@ -2353,7 +2401,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="10" t="s">
         <v>25</v>
       </c>
@@ -2379,7 +2427,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="11">
         <v>100</v>
       </c>
@@ -2405,7 +2453,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="12">
         <v>75</v>
       </c>
@@ -2431,7 +2479,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="11">
         <v>60</v>
       </c>
@@ -2457,7 +2505,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A41" s="12">
         <v>50</v>
       </c>
@@ -2483,7 +2531,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="11">
         <v>0</v>
       </c>
@@ -2509,7 +2557,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G43" s="11">
         <v>25</v>
       </c>
@@ -2523,7 +2571,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G44" s="13">
         <v>30</v>
       </c>
@@ -2537,7 +2585,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G45" s="11">
         <v>35</v>
       </c>
@@ -2551,7 +2599,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G46" s="13">
         <v>40</v>
       </c>
@@ -2565,7 +2613,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G47" s="11">
         <v>45</v>
       </c>
@@ -2579,7 +2627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G48" s="13">
         <v>50</v>
       </c>
@@ -2587,7 +2635,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G49" s="11">
         <v>55</v>
       </c>
@@ -2595,7 +2643,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="50" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G50" s="13">
         <v>60</v>
       </c>
@@ -2603,7 +2651,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="51" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G51" s="11">
         <v>65</v>
       </c>
@@ -2611,7 +2659,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="52" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G52" s="13">
         <v>70</v>
       </c>
@@ -2619,7 +2667,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="53" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G53" s="11">
         <v>75</v>
       </c>
@@ -2627,7 +2675,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G54" s="13">
         <v>80</v>
       </c>
@@ -2635,7 +2683,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G55" s="11">
         <v>85</v>
       </c>
@@ -2643,7 +2691,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="7:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="7:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2652,16 +2700,101 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB089DF1-9149-4C20-B4B4-0C866A8CD97C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="22">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="23">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B8" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8">
+        <f>-0.029*9.81*$C$5/(8.31*(273.15+$C$7))</f>
+        <v>-1.9269037733420934E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9">
+        <f>EXP(C8)</f>
+        <v>0.98091542347744443</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="25">
+        <f>C6*C9</f>
+        <v>745.49572184285773</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <f>EXP(-0.029*9.81/(8.31*(273.15+$C$7)))</f>
+        <v>0.99988322477188862</v>
+      </c>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <f>C13^C5</f>
+        <v>0.98091542347744642</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[WeatherStation] HTML update v2.5b [20200914] - favicon  - bug fix for waning crescent mooon
</commit_message>
<xml_diff>
--- a/WeatherStation2_webserver/WeatherStation.xlsx
+++ b/WeatherStation2_webserver/WeatherStation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="38618" windowHeight="21218" activeTab="4"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="38618" windowHeight="21218" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wire (test)" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
   <si>
     <t>Electrical Parameters</t>
   </si>
@@ -112,9 +112,6 @@
     <t>3.3-5V</t>
   </si>
   <si>
-    <t>Capacitive RainSensor</t>
-  </si>
-  <si>
     <t>thermistor</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>Capacitive</t>
   </si>
   <si>
-    <t>Resistance RainSensor (?)</t>
-  </si>
-  <si>
     <t>BH1750</t>
   </si>
   <si>
@@ -378,6 +372,30 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>Коробка</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>DHT</t>
+  </si>
+  <si>
+    <t>1W</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>3.3v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistance RainSensor </t>
+  </si>
+  <si>
+    <t>Capacitive RainSensor (?)</t>
   </si>
 </sst>
 </file>
@@ -387,7 +405,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,8 +484,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +548,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -550,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -599,6 +631,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1301,6 +1342,363 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13206413" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13444538" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14501813" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13925551" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14397038" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14635163" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15111413" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15368589" y="361950"/>
+          <a:ext cx="0" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1365,7 +1763,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1738,7 +2136,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -1746,10 +2144,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -1757,7 +2155,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1769,10 +2167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1781,17 +2179,21 @@
     <col min="2" max="2" width="13.265625" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="22.9296875" customWidth="1"/>
+    <col min="17" max="17" width="3.796875" customWidth="1"/>
+    <col min="18" max="18" width="3.33203125" customWidth="1"/>
+    <col min="19" max="19" width="4" customWidth="1"/>
+    <col min="20" max="30" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B1" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
@@ -1800,30 +2202,30 @@
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>64</v>
+      <c r="D2" s="26" t="s">
+        <v>98</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J2" s="4"/>
       <c r="L2" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1838,24 +2240,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
       <c r="G4" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1863,393 +2265,453 @@
         <v>9</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5">
+        <v>63</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="28">
         <v>3</v>
       </c>
-      <c r="I5" t="s">
-        <v>69</v>
+      <c r="I5" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="K5">
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="28">
         <v>4</v>
       </c>
-      <c r="I6" t="s">
-        <v>70</v>
+      <c r="I6" s="28" t="s">
+        <v>68</v>
       </c>
       <c r="K6">
         <v>4</v>
       </c>
       <c r="L6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="G7" s="17">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
       <c r="G8" s="17">
         <v>1</v>
       </c>
       <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="17">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="I8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="I10" s="4" t="s">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="H11">
+      <c r="K12">
         <v>1</v>
       </c>
-      <c r="I11" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="I12" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12">
+      <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13">
         <v>2</v>
       </c>
-      <c r="L12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
-        <v>80</v>
-      </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
       <c r="L13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15">
+        <v>3.3</v>
+      </c>
+      <c r="S15" s="29">
+        <v>3.3</v>
+      </c>
+      <c r="T15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="V15" t="s">
+        <v>99</v>
+      </c>
+      <c r="W15" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>57</v>
       </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-      <c r="I15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="H16">
-        <v>6</v>
-      </c>
-      <c r="I16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" t="s">
-        <v>77</v>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21" t="s">
-        <v>72</v>
-      </c>
-      <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="L21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22">
-        <v>3</v>
-      </c>
-      <c r="L22" t="s">
-        <v>69</v>
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23">
-        <v>4</v>
-      </c>
-      <c r="I23" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23">
-        <v>4</v>
-      </c>
-      <c r="L23" t="s">
-        <v>70</v>
+        <v>13</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="K24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
       <c r="H25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H26">
-        <v>7</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>78</v>
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>67</v>
       </c>
       <c r="K26">
-        <v>7</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>87</v>
+        <v>3</v>
+      </c>
+      <c r="L26" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="20" t="s">
-        <v>84</v>
+      <c r="A27" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="H27">
-        <v>8</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>79</v>
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>68</v>
       </c>
       <c r="K27">
-        <v>8</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>75</v>
+        <v>4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H28">
-        <v>9</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>80</v>
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+      <c r="L28" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
       <c r="H29">
-        <v>10</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>81</v>
+        <v>6</v>
+      </c>
+      <c r="I29" t="s">
+        <v>71</v>
+      </c>
+      <c r="K29">
+        <v>6</v>
+      </c>
+      <c r="L29" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="K30">
+        <v>7</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31">
+        <v>8</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32">
+        <v>9</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H34">
         <v>11</v>
       </c>
-      <c r="I30" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="H31">
+      <c r="I34" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H35">
         <v>12</v>
       </c>
-      <c r="I31" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="H32">
+      <c r="I35" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H36">
         <v>13</v>
       </c>
-      <c r="I32" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H33">
+      <c r="I36" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H37">
         <v>14</v>
       </c>
-      <c r="I33" s="16" t="s">
-        <v>75</v>
+      <c r="I37" s="16" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2309,7 +2771,7 @@
     </row>
     <row r="15" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="4">
         <v>3.3</v>
@@ -2326,7 +2788,7 @@
     </row>
     <row r="16" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" s="6">
         <f>J15^2/42</f>
@@ -2347,7 +2809,7 @@
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J17" s="5">
         <f>J16/J15*1000</f>
@@ -2368,63 +2830,63 @@
     </row>
     <row r="35" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="72" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="G36" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H36" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="M36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N36" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="N36" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="G37" s="11">
         <v>-5</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M37" s="11">
         <v>0</v>
       </c>
       <c r="N37" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2432,25 +2894,25 @@
         <v>100</v>
       </c>
       <c r="B38" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="D38" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G38" s="12">
         <v>0</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M38" s="12">
         <v>15</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2458,25 +2920,25 @@
         <v>75</v>
       </c>
       <c r="B39" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="D39" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="G39" s="11">
         <v>5</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M39" s="11">
         <v>30</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2484,25 +2946,25 @@
         <v>60</v>
       </c>
       <c r="B40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="G40" s="12">
         <v>10</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M40" s="12">
         <v>45</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2510,25 +2972,25 @@
         <v>50</v>
       </c>
       <c r="B41" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="D41" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="G41" s="11">
         <v>15</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M41" s="11">
         <v>60</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2536,13 +2998,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="G42" s="13">
         <v>20</v>
@@ -2718,7 +3180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2726,12 +3188,12 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" s="22">
         <v>165</v>
@@ -2739,7 +3201,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C6" s="23">
         <v>760</v>
@@ -2747,7 +3209,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="23">
         <v>20</v>
@@ -2755,7 +3217,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8">
         <f>-0.029*9.81*$C$5/(8.31*(273.15+$C$7))</f>
@@ -2764,7 +3226,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <f>EXP(C8)</f>
@@ -2773,7 +3235,7 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="25">
         <f>C6*C9</f>

</xml_diff>

<commit_message>
[WeatherStatoin]  Old commit? Need before merge
</commit_message>
<xml_diff>
--- a/WeatherStation2_webserver/WeatherStation.xlsx
+++ b/WeatherStation2_webserver/WeatherStation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WeatherStation2_webserver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B258420-99D3-4529-AAA4-C76B3F79CC00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BB0382-B95E-4A13-A631-8CCC25FF5BEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B0C9A41E-2C7E-4A7A-8B40-CD68F4668925}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="list" sheetId="2" r:id="rId2"/>
     <sheet name="Capacitive Rain" sheetId="1" r:id="rId3"/>
     <sheet name="mlx" sheetId="3" r:id="rId4"/>
+    <sheet name="moon icons" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="123">
   <si>
     <t>Electrical Parameters</t>
   </si>
@@ -358,13 +359,104 @@
   <si>
     <t>Test wire diagram</t>
   </si>
+  <si>
+    <t>wi-moon-alt-waning-crescent-6</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-crescent-5</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-crescent-4</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-crescent-3</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-crescent-2</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-crescent-1</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-third-quarter</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-gibbous-6</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-gibbous-5</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-gibbous-4</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-gibbous-3</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-gibbous-2</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waning-gibbous-1</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-full</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-gibbous-6</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-gibbous-5</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-gibbous-4</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-gibbous-3</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-gibbous-2</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-gibbous-1</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-first-quarter</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-crescent-6</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-crescent-5</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-crescent-4</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-crescent-3</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-crescent-2</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-waxing-crescent-1</t>
+  </si>
+  <si>
+    <t>wi-moon-alt-new</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>DB18b20</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -507,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -551,6 +643,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1248,6 +1344,727 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Прямоугольник: скругленные углы 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49D827B3-28CA-4FE9-9264-B41F8E1765F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2578100"/>
+          <a:ext cx="1219200" cy="1473200"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Прямая соединительная линия 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90879524-638A-4088-8A53-2A7441D0E0D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="819150" y="4051300"/>
+          <a:ext cx="0" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>465667</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>465667</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Прямая соединительная линия 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4012282E-9BD9-4A07-BC3C-0B60709B3725}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1075267" y="4051300"/>
+          <a:ext cx="0" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Прямая соединительная линия 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9775E8D7-F77A-4B23-99E5-1B8CA5F83C11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1587500" y="4051300"/>
+          <a:ext cx="0" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>112184</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>112184</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Прямая соединительная линия 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F45F9FF9-4A67-4534-94AE-2A854B7C9F7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1331384" y="4051300"/>
+          <a:ext cx="0" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Прямая соединительная линия 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDCE3AC2-5D9E-4C2A-858D-0089311954A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="819150" y="4787900"/>
+          <a:ext cx="1413510" cy="1289050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Прямая соединительная линия 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{955A4474-DD97-461A-B41A-3A210D1DE9AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066800" y="4787900"/>
+          <a:ext cx="1211580" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:prstDash val="sysDot"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>553720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Прямая соединительная линия 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0FE8E27-56CA-4C56-8145-5134211A3A40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1574800" y="4787900"/>
+          <a:ext cx="807720" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:prstDash val="lgDashDot"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Прямоугольник 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D3AB1CF-DB73-4046-BAF2-DF9BF1E516F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="6445250"/>
+          <a:ext cx="609600" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>602639</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>125106</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>26007</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>135241</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Хорда 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CB14C7F-9344-4C56-8B2B-5ECE056D36BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="7359069">
+          <a:off x="1252230" y="6162065"/>
+          <a:ext cx="562585" cy="642568"/>
+        </a:xfrm>
+        <a:prstGeom prst="chord">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 3936991"/>
+            <a:gd name="adj2" fmla="val 13734126"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Прямая соединительная линия 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3877102A-CBFA-4B24-BE4E-BCD6BA3E5A45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1308100" y="6997700"/>
+          <a:ext cx="0" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Прямая соединительная линия 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{006BC760-9810-422E-99D4-1BDF0588555A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1511300" y="6991350"/>
+          <a:ext cx="0" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Прямая соединительная линия 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D53684-7142-4A45-9ABB-C1EEE3717CCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="6991350"/>
+          <a:ext cx="0" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1680,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FE82ED-A626-4C51-9541-F900C0D39745}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1710,6 +2527,32 @@
       </c>
       <c r="E9" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2664,4 +3507,353 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CD897C-674D-47CF-9305-A9B0E2D4406A}">
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21">
+        <f>A1</f>
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1">
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="M1">
+        <v>3.56E-2</v>
+      </c>
+      <c r="O1">
+        <f>M1/0.035714</f>
+        <v>0.99680797446379565</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B2" s="21">
+        <f>B1+$J$1</f>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="O2">
+        <f>M2/0.035714</f>
+        <v>1.002408019264154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B3" s="21">
+        <f>B2+$J$1</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3">
+        <f>M3/0.035714</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B4" s="21">
+        <f>B3+$J$1</f>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4">
+        <v>0.432</v>
+      </c>
+      <c r="N4">
+        <v>0.25</v>
+      </c>
+      <c r="O4">
+        <f>(M4-N4)/0.035714</f>
+        <v>5.0960407683261462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5" s="21">
+        <f>B4+$J$1</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
+      <c r="O5">
+        <f>M5/0.035714</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B6" s="21">
+        <f>B5+$J$1</f>
+        <v>0.17857142857142855</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="O6">
+        <f>M6/0.035714</f>
+        <v>4.7880383043064345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B7" s="21">
+        <f>B6+$J$1</f>
+        <v>0.21428571428571425</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0.25</v>
+      </c>
+      <c r="B8" s="21">
+        <f>B7+$J$1</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B9" s="21">
+        <f>B8+$J$1</f>
+        <v>0.28571428571428564</v>
+      </c>
+      <c r="F9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" s="21">
+        <f>B9+$J$1</f>
+        <v>0.32142857142857134</v>
+      </c>
+      <c r="F10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B11" s="21">
+        <f>B10+$J$1</f>
+        <v>0.35714285714285704</v>
+      </c>
+      <c r="F11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B12" s="21">
+        <f>B11+$J$1</f>
+        <v>0.39285714285714274</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B13" s="21">
+        <f>B12+$J$1</f>
+        <v>0.42857142857142844</v>
+      </c>
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B14" s="21">
+        <f>B13+$J$1</f>
+        <v>0.46428571428571414</v>
+      </c>
+      <c r="F14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0.5</v>
+      </c>
+      <c r="B15" s="21">
+        <f>B14+$J$1</f>
+        <v>0.49999999999999983</v>
+      </c>
+      <c r="F15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B16" s="21">
+        <f>B15+$J$1</f>
+        <v>0.53571428571428559</v>
+      </c>
+      <c r="F16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="21">
+        <f>B16+$J$1</f>
+        <v>0.57142857142857129</v>
+      </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="21">
+        <f>B17+$J$1</f>
+        <v>0.60714285714285698</v>
+      </c>
+      <c r="F18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="21">
+        <f>B18+$J$1</f>
+        <v>0.64285714285714268</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="21">
+        <f>B19+$J$1</f>
+        <v>0.67857142857142838</v>
+      </c>
+      <c r="F20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="21">
+        <f>B20+$J$1</f>
+        <v>0.71428571428571408</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.75</v>
+      </c>
+      <c r="B22" s="21">
+        <f>B21+$J$1</f>
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="21">
+        <f>B22+$J$1</f>
+        <v>0.78571428571428548</v>
+      </c>
+      <c r="F23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="21">
+        <f>B23+$J$1</f>
+        <v>0.82142857142857117</v>
+      </c>
+      <c r="F24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="21">
+        <f>B24+$J$1</f>
+        <v>0.85714285714285687</v>
+      </c>
+      <c r="F25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="21">
+        <f>B25+$J$1</f>
+        <v>0.89285714285714257</v>
+      </c>
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="21">
+        <f>B26+$J$1</f>
+        <v>0.92857142857142827</v>
+      </c>
+      <c r="F27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="21">
+        <f>B27+$J$1</f>
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="21">
+        <f>B28+$J$1</f>
+        <v>0.99999999999999967</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[WeatherStation] ver 2.3b some debug output for narodmon
</commit_message>
<xml_diff>
--- a/WeatherStation2_webserver/WeatherStation.xlsx
+++ b/WeatherStation2_webserver/WeatherStation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WeatherStation2_webserver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABC30F4-A27D-4706-8F91-89371480FA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9DAB82-08CB-4540-BC6A-1B4F0062A411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,7 +579,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,8 +694,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -798,11 +810,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -904,8 +980,20 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1705,13 +1793,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>39414</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>23587</xdr:rowOff>
+      <xdr:rowOff>10887</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>134069</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>183696</xdr:rowOff>
+      <xdr:rowOff>170996</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1767,13 +1855,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>128376</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>144237</xdr:rowOff>
+      <xdr:rowOff>131537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>32907</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>55556</xdr:rowOff>
+      <xdr:rowOff>42856</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1827,13 +1915,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>103195</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>81175</xdr:rowOff>
+      <xdr:rowOff>68475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>39476</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>30375</xdr:rowOff>
+      <xdr:rowOff>17675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1889,13 +1977,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>102757</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>81175</xdr:rowOff>
+      <xdr:rowOff>68475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>39038</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>30375</xdr:rowOff>
+      <xdr:rowOff>17675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1949,13 +2037,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>103195</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>145113</xdr:rowOff>
+      <xdr:rowOff>132413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>39476</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>94531</xdr:rowOff>
+      <xdr:rowOff>81831</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2009,13 +2097,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>102757</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>145113</xdr:rowOff>
+      <xdr:rowOff>132413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>39038</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>94531</xdr:rowOff>
+      <xdr:rowOff>81831</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4884,7 +4972,7 @@
       <xdr:col>93</xdr:col>
       <xdr:colOff>187013</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>141287</xdr:rowOff>
+      <xdr:rowOff>134937</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6077,7 +6165,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12058659" y="7085012"/>
+          <a:off x="12058659" y="7097712"/>
           <a:ext cx="100004" cy="239712"/>
           <a:chOff x="6319267" y="15462250"/>
           <a:chExt cx="59529" cy="238125"/>
@@ -6327,13 +6415,13 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="28575">
+        <a:ln w="28575" cmpd="dbl">
           <a:solidFill>
             <a:schemeClr val="bg1">
               <a:lumMod val="75000"/>
             </a:schemeClr>
           </a:solidFill>
-          <a:prstDash val="lgDash"/>
+          <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -6730,10 +6818,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>59</xdr:col>
@@ -6754,19 +6842,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10750550" y="3606800"/>
-          <a:ext cx="984251" cy="3663950"/>
+          <a:off x="9931400" y="3581400"/>
+          <a:ext cx="1803401" cy="3689350"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="7030A0"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="solid"/>
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -6790,8 +6876,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
@@ -6799,7 +6885,7 @@
       <xdr:col>59</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6814,19 +6900,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10731500" y="3028950"/>
-          <a:ext cx="1022350" cy="755650"/>
+          <a:off x="9937750" y="3028950"/>
+          <a:ext cx="1816100" cy="774700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="0070C0"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="solid"/>
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -6919,10 +7003,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>91</xdr:col>
@@ -6945,20 +7029,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10725150" y="3956050"/>
-          <a:ext cx="7308538" cy="3612200"/>
+          <a:off x="9912350" y="3949700"/>
+          <a:ext cx="8121338" cy="3618550"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
+            <a:srgbClr val="0070C0"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="solid"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -6981,10 +7062,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>146050</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>58</xdr:col>
@@ -7005,19 +7086,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10775950" y="3232150"/>
-          <a:ext cx="768350" cy="1847850"/>
+          <a:off x="9956800" y="3175000"/>
+          <a:ext cx="1587500" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="00B050"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="solid"/>
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -7041,10 +7120,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>58</xdr:col>
@@ -7065,19 +7144,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10744200" y="3390900"/>
-          <a:ext cx="768350" cy="1847850"/>
+          <a:off x="9925050" y="3384550"/>
+          <a:ext cx="1587500" cy="1854200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="FFFF00"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="solid"/>
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -7101,10 +7178,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
@@ -7125,19 +7202,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10750550" y="2825750"/>
-          <a:ext cx="1962150" cy="1104900"/>
+          <a:off x="9931400" y="2838450"/>
+          <a:ext cx="2781300" cy="1092200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="FF0000"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="solid"/>
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -7161,10 +7236,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>63</xdr:col>
@@ -7185,19 +7260,17 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10731500" y="2984500"/>
-          <a:ext cx="1746250" cy="939800"/>
+          <a:off x="9906000" y="3022600"/>
+          <a:ext cx="2571750" cy="901700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="FFC000"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="solid"/>
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -7211,6 +7284,236 @@
         </a:fillRef>
         <a:effectRef idx="2">
           <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Прямая соединительная линия 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097FACE8-030D-47CA-AF59-AAEA2762E95C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3676650" y="4502150"/>
+          <a:ext cx="984250" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="118" name="Прямая соединительная линия 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59DC17DF-5299-4165-A08F-737C85E03EE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3854450" y="4603750"/>
+          <a:ext cx="1968500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="133" name="Прямая соединительная линия 132">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C5E39B-BD22-4993-AECB-4BAB8978F299}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235450" y="4660900"/>
+          <a:ext cx="1987550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050" cmpd="dbl">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="138" name="Прямая соединительная линия 137">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA2263B1-0E36-4FD6-B42E-798DB6D057A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4064000" y="4730750"/>
+          <a:ext cx="393700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -14696,7 +14999,7 @@
   <dimension ref="B7:BJ52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BT14" sqref="BT14"/>
+      <selection activeCell="AL38" sqref="AL38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14860,183 +15163,148 @@
       </c>
     </row>
     <row r="24" spans="19:62" x14ac:dyDescent="0.35">
+      <c r="S24" t="s">
+        <v>123</v>
+      </c>
+      <c r="W24" t="s">
+        <v>122</v>
+      </c>
       <c r="BD24">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="S25" t="s">
-        <v>123</v>
-      </c>
-      <c r="W25" t="s">
-        <v>122</v>
-      </c>
+      <c r="S25" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="T25" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="U25" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="V25" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="W25" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="X25" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y25" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z25" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA25" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB25" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC25" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD25" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE25" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF25" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG25" s="69"/>
       <c r="BD25">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="S26" s="66" t="s">
-        <v>114</v>
-      </c>
-      <c r="T26" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="U26" s="66" t="s">
-        <v>121</v>
-      </c>
-      <c r="V26" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="W26" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="X26" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y26" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z26" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA26" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB26" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC26" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD26" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE26" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF26" s="62" t="s">
-        <v>120</v>
-      </c>
+    <row r="26" spans="19:62" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S26" s="65"/>
+      <c r="T26" s="66"/>
+      <c r="U26" s="66"/>
+      <c r="V26" s="66"/>
+      <c r="W26" s="67"/>
+      <c r="X26" s="68"/>
+      <c r="Y26" s="68"/>
+      <c r="Z26" s="68"/>
+      <c r="AA26" s="68"/>
+      <c r="AB26" s="68"/>
+      <c r="AC26" s="68"/>
+      <c r="AD26" s="67"/>
+      <c r="AE26" s="67"/>
+      <c r="AF26" s="68"/>
+      <c r="AG26" s="69"/>
       <c r="BD26">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="S27" s="66" t="s">
+    <row r="27" spans="19:62" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="S27" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="T27" s="66" t="s">
+      <c r="T27" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="U27" s="66" t="s">
+      <c r="U27" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="V27" s="66"/>
-      <c r="W27" s="65" t="s">
+      <c r="V27" s="72"/>
+      <c r="W27" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="X27" s="62" t="s">
+      <c r="X27" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="Y27" s="62" t="s">
+      <c r="Y27" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="Z27" s="62" t="s">
+      <c r="Z27" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="AA27" s="62" t="s">
+      <c r="AA27" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="AB27" s="62" t="s">
+      <c r="AB27" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="AC27" s="62" t="s">
+      <c r="AC27" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="AD27" s="65" t="s">
+      <c r="AD27" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="AE27" s="65" t="s">
+      <c r="AE27" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="AF27" s="62"/>
+      <c r="AF27" s="75"/>
+      <c r="AG27" s="76"/>
       <c r="BD27">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="S28">
-        <v>1</v>
-      </c>
-      <c r="T28">
-        <f>S28+1</f>
-        <v>2</v>
-      </c>
-      <c r="U28">
-        <f t="shared" ref="U28:AI28" si="1">T28+1</f>
-        <v>3</v>
-      </c>
-      <c r="V28">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="W28">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="X28">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="Y28">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="Z28">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AA28">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="AB28">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="AC28">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="AD28">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="AE28">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="AF28">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="AG28">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="AH28">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="AI28">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
+      <c r="S28" s="65"/>
+      <c r="T28" s="66"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="77"/>
+      <c r="W28" s="67"/>
+      <c r="X28" s="68"/>
+      <c r="Y28" s="68"/>
+      <c r="Z28" s="68"/>
+      <c r="AA28" s="68"/>
+      <c r="AB28" s="68"/>
+      <c r="AC28" s="68"/>
+      <c r="AD28" s="67"/>
+      <c r="AE28" s="67"/>
+      <c r="AF28" s="78"/>
+      <c r="AG28" s="69"/>
       <c r="BD28">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -15050,6 +15318,64 @@
       <c r="BJ28" s="38"/>
     </row>
     <row r="29" spans="19:62" x14ac:dyDescent="0.35">
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <f>S29+1</f>
+        <v>2</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ref="U29:AI29" si="1">T29+1</f>
+        <v>3</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AB29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="AG29">
+        <v>15</v>
+      </c>
       <c r="BD29">
         <f t="shared" si="0"/>
         <v>17</v>

</xml_diff>

<commit_message>
[WeatherStation]  ver 2.4с 2020/11/02 [454744/32904]                       - moving to narodmon GET sending failed and left POST with some modifications
</commit_message>
<xml_diff>
--- a/WeatherStation2_webserver/WeatherStation.xlsx
+++ b/WeatherStation2_webserver/WeatherStation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WeatherStation2_webserver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9DAB82-08CB-4540-BC6A-1B4F0062A411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD432D8-6740-4C3C-AAD7-857CB71C58F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="132">
   <si>
     <t>Electrical Parameters</t>
   </si>
@@ -474,6 +474,12 @@
   <si>
     <t>j</t>
   </si>
+  <si>
+    <t>5v</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
 </sst>
 </file>
 
@@ -702,7 +708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -878,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -987,13 +993,10 @@
     <xf numFmtId="0" fontId="10" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2483,9 +2486,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>97378</xdr:rowOff>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2501,7 +2504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1181100" y="1841500"/>
-          <a:ext cx="3232150" cy="3043778"/>
+          <a:ext cx="3257550" cy="3181350"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2538,9 +2541,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2556,7 +2559,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1574800" y="1841500"/>
-          <a:ext cx="3251200" cy="3041650"/>
+          <a:ext cx="3270250" cy="3187700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2592,10 +2595,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2611,7 +2614,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="984250" y="1841500"/>
-          <a:ext cx="3848100" cy="2844800"/>
+          <a:ext cx="5194300" cy="3155950"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2648,9 +2651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2666,7 +2669,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3346450" y="2393950"/>
-          <a:ext cx="1257300" cy="2476500"/>
+          <a:ext cx="1276350" cy="2552700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5857,16 +5860,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>61</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>64</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5880,9 +5883,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="4419600" y="11322050"/>
-          <a:ext cx="571500" cy="882650"/>
+        <a:xfrm flipV="1">
+          <a:off x="9550400" y="2851150"/>
+          <a:ext cx="2546350" cy="889000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5977,7 +5980,7 @@
     <xdr:to>
       <xdr:col>91</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>136318</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5990,13 +5993,13 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:endCxn id="164" idx="2"/>
+          <a:endCxn id="163" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4438650" y="11512550"/>
-          <a:ext cx="5905500" cy="3724068"/>
+          <a:off x="12115800" y="3041650"/>
+          <a:ext cx="5905500" cy="3184318"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6819,15 +6822,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>59</xdr:col>
       <xdr:colOff>120651</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6841,9 +6844,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9931400" y="3581400"/>
-          <a:ext cx="1803401" cy="3689350"/>
+        <a:xfrm flipV="1">
+          <a:off x="9874250" y="7283450"/>
+          <a:ext cx="1860551" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7004,8 +7007,8 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -7029,8 +7032,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9912350" y="3949700"/>
-          <a:ext cx="8121338" cy="3618550"/>
+          <a:off x="9931400" y="7092950"/>
+          <a:ext cx="8102288" cy="488000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7040,6 +7043,7 @@
             <a:srgbClr val="0070C0"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -7063,14 +7067,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>58</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7085,9 +7089,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9956800" y="3175000"/>
-          <a:ext cx="1587500" cy="1905000"/>
+        <a:xfrm flipV="1">
+          <a:off x="9931400" y="5092700"/>
+          <a:ext cx="1612900" cy="2762250"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7121,15 +7125,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>58</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7143,9 +7147,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9925050" y="3384550"/>
-          <a:ext cx="1587500" cy="1854200"/>
+        <a:xfrm flipV="1">
+          <a:off x="9906000" y="5251450"/>
+          <a:ext cx="1606550" cy="2432050"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7179,15 +7183,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>64</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7201,9 +7205,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9931400" y="2838450"/>
-          <a:ext cx="2781300" cy="1092200"/>
+        <a:xfrm flipV="1">
+          <a:off x="9956800" y="3930650"/>
+          <a:ext cx="2755900" cy="4292600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7237,15 +7241,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>63</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7259,9 +7263,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9906000" y="3022600"/>
-          <a:ext cx="2571750" cy="901700"/>
+        <a:xfrm flipV="1">
+          <a:off x="9944100" y="3924300"/>
+          <a:ext cx="2533650" cy="4114800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7503,6 +7507,1285 @@
           </a:solidFill>
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="141" name="Прямая соединительная линия 140">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D20F7F5-322B-48C7-A4F8-7970510CC875}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3822700" y="4997450"/>
+          <a:ext cx="2019300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050" cmpd="dbl">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="142" name="Прямая соединительная линия 141">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA713CA-616E-4504-80D2-2524EEC30AAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4171950" y="5086350"/>
+          <a:ext cx="2019300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="168" name="Прямая соединительная линия 167">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D3E452E-E7B6-4B90-B6B3-5592D9CCD083}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="4870450"/>
+          <a:ext cx="1073150" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="169" name="Прямая соединительная линия 168">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{488747F0-AC5D-42FD-BB5E-F6A8B149AE9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4006850" y="5130800"/>
+          <a:ext cx="450850" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="170" name="Прямоугольник: усеченные верхние углы 169">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{804ABF2D-060A-4FDD-91E8-103AD3391CDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3149600" y="8470900"/>
+          <a:ext cx="984250" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>DHT22</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="171" name="Прямая со стрелкой 170">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8007E59D-5544-4437-9DC6-8E92E4BB4DC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3346450" y="9575800"/>
+          <a:ext cx="0" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="172" name="Прямая со стрелкой 171">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6058D1DB-FECC-4E4E-9C69-E1E5CF7E4048}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3543300" y="9575800"/>
+          <a:ext cx="0" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="173" name="Прямая со стрелкой 172">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64654978-F3AF-4E89-91DC-1D0E4ABCCE8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3740150" y="9575800"/>
+          <a:ext cx="0" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="174" name="Прямая со стрелкой 173">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D23DD9F3-9615-4D29-8A9D-DE654D588892}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3937000" y="9575800"/>
+          <a:ext cx="0" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="175" name="Прямая со стрелкой 174">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFD5756E-A7A3-42A9-A2C3-27B7E18B6D8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7677150" y="1841500"/>
+          <a:ext cx="0" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="176" name="Прямая со стрелкой 175">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD60FEA5-0B7C-4D7B-AED6-4CA1877F5F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7874000" y="1841500"/>
+          <a:ext cx="0" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="177" name="Прямая со стрелкой 176">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA297BA1-BB50-4579-A4A1-002DE5E6E574}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8070850" y="2025650"/>
+          <a:ext cx="0" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="lgDashDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="178" name="Прямая со стрелкой 177">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5D82465-535D-4D4E-834E-BC2CEFFA7D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3740150" y="9759950"/>
+          <a:ext cx="203200" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="lgDashDot"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="179" name="Прямая со стрелкой 178">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDC87392-299D-46DF-B6AD-B2733198F5DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7677150" y="2876550"/>
+          <a:ext cx="3657600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="194" name="Прямая со стрелкой 193">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F759509C-A83E-41E9-BB7C-CDE8DA0DA158}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7874000" y="3060700"/>
+          <a:ext cx="3467100" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="195" name="Прямая со стрелкой 194">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D85433A-6131-4C55-B49A-42F38D2BD9BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8070850" y="3244850"/>
+          <a:ext cx="3282950" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="lgDashDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="198" name="Прямоугольник 197">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{263E646A-861F-46B3-AC10-AA7926B5C70B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9448800" y="2762250"/>
+          <a:ext cx="196850" cy="5537200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="10196"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="199" name="Прямая соединительная линия 198">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBF11BC5-F7DC-4A0A-B6E3-796DCE0170C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9912350" y="2870200"/>
+          <a:ext cx="234950" cy="4451350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>136318</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="201" name="Прямая соединительная линия 200">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8412A348-40E0-46BC-9C8D-BCCA8AFCDCA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="164" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10293350" y="2901950"/>
+          <a:ext cx="7727950" cy="3876468"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575" cmpd="dbl">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>102416</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180185</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>76221</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>96039</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="204" name="Группа 203">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{853D6447-69B0-4B07-8341-56F6CBA94D30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm rot="16200000">
+          <a:off x="9684967" y="2624534"/>
+          <a:ext cx="100004" cy="367505"/>
+          <a:chOff x="6326827" y="15462250"/>
+          <a:chExt cx="59529" cy="365070"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="205" name="Прямая соединительная линия 204">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01BF764-7B8C-4046-A0AC-DB2EB7CD7F5E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000" flipV="1">
+            <a:off x="6169343" y="15642907"/>
+            <a:ext cx="365070" cy="3756"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="207" name="Прямоугольник: скругленные углы 206">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC4B940-3D58-4EB7-BE9A-AABD5BE10D7A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="6285284" y="15638142"/>
+            <a:ext cx="142616" cy="59529"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ru-RU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="210" name="Прямая со стрелкой 209">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80E773D9-31AE-4DFA-B73E-C0298FD123CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9499600" y="6908800"/>
+          <a:ext cx="406400" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -14996,22 +16279,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1024DC6-371D-49B7-B8D4-D735C98C1199}">
-  <dimension ref="B7:BJ52"/>
+  <dimension ref="B7:BK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL38" sqref="AL38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC38" sqref="BC38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="7" spans="5:62" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:63" x14ac:dyDescent="0.35">
       <c r="BD7" s="34"/>
       <c r="BE7" s="34"/>
       <c r="BF7" s="34"/>
       <c r="BG7" s="34"/>
       <c r="BH7" s="34"/>
     </row>
-    <row r="9" spans="5:62" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:63" x14ac:dyDescent="0.35">
       <c r="P9" s="34"/>
       <c r="Q9" s="34" t="s">
         <v>113</v>
@@ -15024,7 +16307,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="5:62" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:63" x14ac:dyDescent="0.35">
       <c r="E10" s="34" t="s">
         <v>114</v>
       </c>
@@ -15036,8 +16319,19 @@
       <c r="I10" s="34" t="s">
         <v>113</v>
       </c>
+      <c r="AM10" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN10" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO10" s="34"/>
+      <c r="AP10" s="34"/>
+      <c r="AQ10" s="34" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="15" spans="5:62" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:63" x14ac:dyDescent="0.35">
       <c r="AY15" t="s">
         <v>129</v>
       </c>
@@ -15069,7 +16363,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="5:62" x14ac:dyDescent="0.35">
+    <row r="16" spans="5:63" x14ac:dyDescent="0.35">
       <c r="Z16" s="34" t="s">
         <v>114</v>
       </c>
@@ -15083,32 +16377,26 @@
       <c r="AD16" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="BC16" s="57" t="s">
-        <v>114</v>
-      </c>
       <c r="BD16">
         <f t="shared" ref="BD16:BD43" si="0">BD17+1</f>
         <v>30</v>
       </c>
-      <c r="BF16" s="32"/>
-      <c r="BG16" s="32"/>
-      <c r="BH16" s="32"/>
-      <c r="BI16" s="32"/>
-      <c r="BJ16" s="32"/>
+      <c r="BF16" s="75"/>
+      <c r="BG16" s="75"/>
+      <c r="BH16" s="75"/>
+      <c r="BI16" s="75"/>
+      <c r="BJ16" s="75"/>
+      <c r="BK16" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="17" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="BC17" s="61" t="s">
-        <v>70</v>
-      </c>
       <c r="BD17">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="BC18" s="58" t="s">
-        <v>67</v>
-      </c>
       <c r="BD18">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -15120,43 +16408,30 @@
       <c r="BJ18" s="33"/>
     </row>
     <row r="19" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="BC19" s="62" t="s">
-        <v>68</v>
-      </c>
       <c r="BD19">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="BC20" s="59" t="s">
-        <v>121</v>
-      </c>
       <c r="BD20">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="BC21" s="63" t="s">
-        <v>100</v>
-      </c>
       <c r="BD21">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="BC22" s="60" t="s">
-        <v>120</v>
-      </c>
       <c r="BD22">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="19:62" x14ac:dyDescent="0.35">
-      <c r="BC23" s="64"/>
       <c r="BD23">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -15254,36 +16529,40 @@
       <c r="U27" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="V27" s="72"/>
-      <c r="W27" s="73" t="s">
+      <c r="V27" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="W27" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="X27" s="74" t="s">
+      <c r="X27" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="Y27" s="74" t="s">
+      <c r="Y27" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="Z27" s="74" t="s">
+      <c r="Z27" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="AA27" s="74" t="s">
+      <c r="AA27" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="AB27" s="74" t="s">
+      <c r="AB27" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="AC27" s="74" t="s">
+      <c r="AC27" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="AD27" s="73" t="s">
+      <c r="AD27" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="AE27" s="73" t="s">
+      <c r="AE27" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="AF27" s="75"/>
-      <c r="AG27" s="76"/>
+      <c r="AF27" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG27" s="74"/>
       <c r="BD27">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -15293,7 +16572,7 @@
       <c r="S28" s="65"/>
       <c r="T28" s="66"/>
       <c r="U28" s="66"/>
-      <c r="V28" s="77"/>
+      <c r="V28" s="66"/>
       <c r="W28" s="67"/>
       <c r="X28" s="68"/>
       <c r="Y28" s="68"/>
@@ -15303,7 +16582,7 @@
       <c r="AC28" s="68"/>
       <c r="AD28" s="67"/>
       <c r="AE28" s="67"/>
-      <c r="AF28" s="78"/>
+      <c r="AF28" s="68"/>
       <c r="AG28" s="69"/>
       <c r="BD28">
         <f t="shared" si="0"/>
@@ -15326,7 +16605,7 @@
         <v>2</v>
       </c>
       <c r="U29">
-        <f t="shared" ref="U29:AI29" si="1">T29+1</f>
+        <f t="shared" ref="U29:AF29" si="1">T29+1</f>
         <v>3</v>
       </c>
       <c r="V29">
@@ -15432,7 +16711,9 @@
       <c r="U32" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="V32" s="64"/>
+      <c r="V32" s="64" t="s">
+        <v>130</v>
+      </c>
       <c r="BD32">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -15469,12 +16750,18 @@
       </c>
     </row>
     <row r="38" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC38" s="64" t="s">
+        <v>131</v>
+      </c>
       <c r="BD38">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC39" s="60" t="s">
+        <v>120</v>
+      </c>
       <c r="BD39">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -15486,12 +16773,18 @@
       <c r="BJ39" s="32"/>
     </row>
     <row r="40" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC40" s="63" t="s">
+        <v>100</v>
+      </c>
       <c r="BD40">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC41" s="59" t="s">
+        <v>121</v>
+      </c>
       <c r="BD41">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -15503,24 +16796,36 @@
       <c r="BJ41" s="33"/>
     </row>
     <row r="42" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC42" s="62" t="s">
+        <v>68</v>
+      </c>
       <c r="BD42">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC43" s="58" t="s">
+        <v>67</v>
+      </c>
       <c r="BD43">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC44" s="61" t="s">
+        <v>70</v>
+      </c>
       <c r="BD44">
         <f>BD45+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="2:62" x14ac:dyDescent="0.35">
+      <c r="BC45" s="57" t="s">
+        <v>114</v>
+      </c>
       <c r="BD45">
         <v>1</v>
       </c>
@@ -16026,8 +17331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F6F37A-738F-4003-BE46-894266D84ACF}">
   <dimension ref="A53:W104"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U101" sqref="U101"/>
+    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44:W59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>